<commit_message>
Fix proof required formula highlight for false fields
</commit_message>
<xml_diff>
--- a/WebsiteCreator/ImageCreators/ImageCreatorTrig.xlsx
+++ b/WebsiteCreator/ImageCreators/ImageCreatorTrig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/491e2628f664332b/Documents_Charl/Computer_Technical/Programming_GitHub/AustralianSchoolMaths/WebsiteCreator/ImageCreators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_F25DC773A252ABDACC10483119D84B8A5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6882C9BB-D695-4B06-B9BA-53C6904BCB5C}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_F25DC773A252ABDACC10483119D84B8A5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B839140-F605-4510-9A86-5F38C108C08F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,13 +104,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -167,7 +167,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>523874</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>98425</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="460376" cy="195759"/>
@@ -319,13 +319,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -369,13 +369,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -419,7 +419,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>574675</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="253467" cy="175369"/>
@@ -583,7 +583,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="253467" cy="175369"/>
@@ -747,13 +747,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -810,13 +810,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -860,13 +860,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>425450</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -910,13 +910,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -960,13 +960,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1010,13 +1010,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>425450</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1060,7 +1060,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>454025</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>79375</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="202620" cy="195759"/>
@@ -1212,7 +1212,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>136525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="253467" cy="175369"/>
@@ -1376,7 +1376,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>511175</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>15875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="253467" cy="175369"/>
@@ -1802,32 +1802,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F62744-82D2-4A3B-A267-D2E377FE4A99}">
-  <dimension ref="D15:F39"/>
+  <dimension ref="D11:F35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="15" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F15">
+    <row r="11" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F11">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="4:5" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="E21" s="1">
+    <row r="16" spans="6:6" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="E17" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D30" s="2">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D26" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D39">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D35">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add sin cos graphs to MA-T1
</commit_message>
<xml_diff>
--- a/WebsiteCreator/ImageCreators/ImageCreatorTrig.xlsx
+++ b/WebsiteCreator/ImageCreators/ImageCreatorTrig.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/491e2628f664332b/Documents_Charl/Computer_Technical/Programming_GitHub/AustralianSchoolMaths/WebsiteCreator/ImageCreators/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive\Documents_Charl\Computer_Technical\Programming_GitHub\AustralianSchoolMaths\WebsiteCreator\ImageCreators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="11_F25DC773A252ABDACC10483119D84B8A5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52D24B1E-6975-4161-8622-B10567DCD84A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B970BD-C69F-4D35-9903-8FF2864FF4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StdAngles" sheetId="8" r:id="rId1"/>
-    <sheet name="GraphData" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
+    <sheet name="Graphs" sheetId="6" r:id="rId2"/>
+    <sheet name="RadianLables" sheetId="11" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
@@ -23,8 +23,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="Max_x_Value" localSheetId="1">GraphData!$C$5</definedName>
-    <definedName name="Min_x_Value" localSheetId="1">GraphData!$C$4</definedName>
+    <definedName name="Max_x_Value" localSheetId="2">RadianLables!#REF!</definedName>
+    <definedName name="Min_x_Value" localSheetId="2">RadianLables!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -69,61 +69,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Graph Data</t>
-  </si>
-  <si>
-    <t>sin</t>
-  </si>
-  <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>Min Value</t>
-  </si>
-  <si>
-    <t>Max Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Radians</t>
   </si>
   <si>
-    <t>Degrees</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>°</t>
+    <t>Trig Graphs</t>
   </si>
   <si>
-    <t>Circle unichar</t>
+    <t>y=sin(x)</t>
   </si>
   <si>
-    <t>Paste special</t>
+    <t>Radian tick lables</t>
   </si>
   <si>
-    <t>Degree symbol  used for formatting</t>
-  </si>
-  <si>
-    <t>Cannot find any literature for drawing tan</t>
-  </si>
-  <si>
-    <t>Dsplaying fractions of pi in radians looks messy and not sure how to set format to display 2 pi and 3/2 pi without reducign to 1 1/2</t>
-  </si>
-  <si>
-    <t>Potentially abort?</t>
+    <t>y=cos(x)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000000000"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00_);\(#,##0.00\);\-??"/>
-    <numFmt numFmtId="184" formatCode="_-* #,##0\°_-;\-* #,##0\°_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,38 +106,8 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -187,11 +130,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -199,44 +141,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="12">
     <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00_);\(#,##0.00\);\-??"/>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="184" formatCode="_-* #,##0\°_-;\-* #,##0\°_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -285,10 +219,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="SpreadsheetBiStyle" pivot="0" table="0" count="4" xr9:uid="{5890DF3A-0ABD-4274-8E00-EB660A947AED}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="firstRowStripe" dxfId="4"/>
-      <tableStyleElement type="secondRowStripe" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="10"/>
+      <tableStyleElement type="firstRowStripe" dxfId="9"/>
+      <tableStyleElement type="secondRowStripe" dxfId="8"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -316,70 +250,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>y = sin(x)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.66021119585281951"/>
-          <c:y val="0.20829315332690454"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -388,23 +259,14 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>GraphData!$E$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>sin</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
+              <a:headEnd type="arrow" w="med" len="med"/>
+              <a:tailEnd type="arrow" w="med" len="med"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -413,180 +275,132 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>GraphData!$D$8:$D$34</c:f>
+              <c:f>Graphs!$B$6:$B$24</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0\°_-;\-* #,##0\°_-;_-* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>-360</c:v>
+                  <c:v>-6.5973445725385655</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-332.30769230769232</c:v>
+                  <c:v>-5.8643062867009474</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-304.61538461538458</c:v>
+                  <c:v>-5.1312680008633285</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-276.92307692307696</c:v>
+                  <c:v>-4.3982297150257104</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-249.23076923076923</c:v>
+                  <c:v>-3.6651914291880918</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-221.53846153846155</c:v>
+                  <c:v>-2.9321531433504733</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-193.84615384615387</c:v>
+                  <c:v>-2.1991148575128552</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-166.15384615384616</c:v>
+                  <c:v>-1.4660765716752362</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-138.46153846153848</c:v>
+                  <c:v>-0.7330382858376181</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-110.76923076923077</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-83.076923076923109</c:v>
+                  <c:v>0.73303828583761899</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-55.384615384615387</c:v>
+                  <c:v>1.466076571675238</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-27.692307692307718</c:v>
+                  <c:v>2.1991148575128552</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2.9321531433504742</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.692307692307669</c:v>
+                  <c:v>3.6651914291880932</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>55.384615384615387</c:v>
+                  <c:v>4.3982297150257104</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>83.076923076923066</c:v>
+                  <c:v>5.1312680008633293</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>110.76923076923077</c:v>
+                  <c:v>5.8643062867009483</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>138.46153846153845</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>166.15384615384613</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>193.84615384615381</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>221.53846153846155</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>249.23076923076923</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>276.92307692307691</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>304.61538461538458</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>332.30769230769226</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>360</c:v>
+                  <c:v>6.5973445725385655</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>GraphData!$E$8:$E$34</c:f>
+              <c:f>Graphs!$C$6:$C$24</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00_);\(#,##0.00\);\-??</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>2.45029690981724E-16</c:v>
+                  <c:v>-0.30901699437494717</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4647231720437684</c:v>
+                  <c:v>0.40673664307580015</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82298386589365657</c:v>
+                  <c:v>0.91354545764260109</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99270887409805397</c:v>
+                  <c:v>0.95105651629515353</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93501624268541472</c:v>
+                  <c:v>0.49999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6631226582407953</c:v>
+                  <c:v>-0.20791169081775973</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23931566428755788</c:v>
+                  <c:v>-0.80901699437494745</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.23931566428755768</c:v>
+                  <c:v>-0.99452189536827329</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.66312265824079519</c:v>
+                  <c:v>-0.66913060635885802</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.93501624268541483</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.99270887409805408</c:v>
+                  <c:v>0.66913060635885868</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.82298386589365646</c:v>
+                  <c:v>0.9945218953682734</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.46472317204376895</c:v>
+                  <c:v>0.80901699437494745</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.20791169081775887</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.46472317204376817</c:v>
+                  <c:v>-0.50000000000000089</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.82298386589365646</c:v>
+                  <c:v>-0.95105651629515353</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.99270887409805397</c:v>
+                  <c:v>-0.91354545764260076</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.93501624268541483</c:v>
+                  <c:v>-0.40673664307579932</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.66312265824079553</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.23931566428755854</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-0.23931566428755657</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-0.6631226582407953</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-0.93501624268541472</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-0.99270887409805408</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-0.82298386589365702</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-0.46472317204376995</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-2.45029690981724E-16</c:v>
+                  <c:v>0.30901699437494717</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -594,7 +408,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-180E-4448-8C7D-656F4582E8CA}"/>
+              <c16:uniqueId val="{00000000-6EF5-4CF0-8ECB-DDB00B26DD02}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -606,20 +420,20 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1673166495"/>
-        <c:axId val="1673172255"/>
+        <c:axId val="201277360"/>
+        <c:axId val="201274480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1673166495"/>
+        <c:axId val="201277360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="_-* #,##0\°_-;\-* #,##0\°_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -630,6 +444,8 @@
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
+            <a:headEnd type="arrow" w="med" len="med"/>
+            <a:tailEnd type="arrow" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -653,24 +469,21 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1673172255"/>
+        <c:crossAx val="201274480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1673172255"/>
+        <c:axId val="201274480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.5"/>
-          <c:min val="-1.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="#,##0.00_);\(#,##0.00\);\-??" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -681,6 +494,8 @@
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
+            <a:headEnd type="arrow" w="med" len="med"/>
+            <a:tailEnd type="arrow" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -704,14 +519,350 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1673166495"/>
+        <c:crossAx val="201277360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Graphs!$B$30:$B$48</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-6.5973445725385655</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.8643062867009474</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.1312680008633285</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.3982297150257104</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.6651914291880918</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.9321531433504733</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.1991148575128552</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.4660765716752362</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.7330382858376181</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.73303828583761899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.466076571675238</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1991148575128552</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.9321531433504742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6651914291880932</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.3982297150257104</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.1312680008633293</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.8643062867009483</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.5973445725385655</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Graphs!$C$30:$C$48</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.95105651629515364</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91354545764260098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.40673664307579976</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.30901699437494756</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.86602540378443882</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.97814760073380558</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.58778525229247303</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10452846326765412</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.74314482547739447</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.74314482547739391</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.10452846326765235</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.58778525229247303</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.97814760073380569</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.86602540378443815</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.30901699437494756</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.40673664307580054</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.91354545764260131</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.95105651629515364</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6EF5-4CF0-8ECB-DDB00B26DD02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="201277360"/>
+        <c:axId val="201274480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="201277360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:headEnd type="arrow" w="med" len="med"/>
+            <a:tailEnd type="arrow" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="201274480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="201274480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:headEnd type="arrow" w="med" len="med"/>
+            <a:tailEnd type="arrow" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="201277360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -801,7 +952,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2768,23 +3475,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>587374</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>98425</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>355599</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>403225</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B128EEE5-97FF-9D0E-5843-ED7A2B0DCFEC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AB0BF6D-74C6-97EB-3420-E4DFFCF49AA8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2802,34 +3509,1727 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>12701</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>431800</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="Picture 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FBC8674-3FAA-823F-5B6F-25C9F593A70F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="RadianLables!$B$11:$J$13" spid="_x0000_s12308"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="3295651" y="2336800"/>
+              <a:ext cx="3467099" cy="488950"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:noFill/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>136525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>441325</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFB18DB5-2ED7-73D7-BCC4-47C9A0C1DF3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>82550</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>50800</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>501649</xdr:colOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Picture 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD2961AD-4612-45CE-88A8-01583DFD747D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="RadianLables!$B$11:$J$13" spid="_x0000_s12309"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="3365500" y="6731000"/>
+              <a:ext cx="3467099" cy="488950"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:noFill/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>739775</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="325538" cy="316882"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{676DD90A-ACAA-441D-AA32-85FABF25033F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1692275" y="479425"/>
+              <a:ext cx="325538" cy="316882"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜋</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{676DD90A-ACAA-441D-AA32-85FABF25033F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1692275" y="479425"/>
+              <a:ext cx="325538" cy="316882"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−3𝜋/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="302006" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7CCCD3D-E290-4E24-A9C9-C242C93F6A08}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="374650" y="2035175"/>
+              <a:ext cx="302006" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100" i="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>2</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜋</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7CCCD3D-E290-4E24-A9C9-C242C93F6A08}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="374650" y="2035175"/>
+              <a:ext cx="302006" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−2𝜋</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="223907" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA599B8-29EB-41A7-BCED-2A3EEC9C5A73}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2717800" y="549275"/>
+              <a:ext cx="223907" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜋</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA599B8-29EB-41A7-BCED-2A3EEC9C5A73}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2717800" y="549275"/>
+              <a:ext cx="223907" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−𝜋</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="247440" cy="287643"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD436E6F-6866-44DB-9BE9-837EE8243889}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3644900" y="517525"/>
+              <a:ext cx="247440" cy="287643"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜋</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD436E6F-6866-44DB-9BE9-837EE8243889}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3644900" y="517525"/>
+              <a:ext cx="247440" cy="287643"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−𝜋/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>863600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="196850" cy="287643"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{971DB0C9-F403-42E0-9989-90EC9A81FB43}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4673600" y="504825"/>
+              <a:ext cx="196850" cy="287643"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜋</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{971DB0C9-F403-42E0-9989-90EC9A81FB43}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4673600" y="504825"/>
+              <a:ext cx="196850" cy="287643"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜋/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>908050</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="118494" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2A9F92-6D1C-4813-92FD-35849558B097}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5670550" y="549275"/>
+              <a:ext cx="118494" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜋</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2A9F92-6D1C-4813-92FD-35849558B097}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5670550" y="549275"/>
+              <a:ext cx="118494" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜋</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>869950</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="196592" cy="316882"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A127C6C8-735A-429B-B439-5ED4FB25E30F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6584950" y="473075"/>
+              <a:ext cx="196592" cy="316882"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜋</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A127C6C8-735A-429B-B439-5ED4FB25E30F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6584950" y="473075"/>
+              <a:ext cx="196592" cy="316882"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>3𝜋/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>850900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="196592" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FAC2A32-3198-419B-896F-2989F78FA3E5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7518400" y="568325"/>
+              <a:ext cx="196592" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>2</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜋</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FAC2A32-3198-419B-896F-2989F78FA3E5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7518400" y="568325"/>
+              <a:ext cx="196592" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>2𝜋</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E56EB970-1AB7-5F63-DD57-6D4B0204332C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="209550" y="635000"/>
+          <a:ext cx="5721350" cy="1155700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100"/>
+            <a:t>Below</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" baseline="0"/>
+            <a:t> radian symbols are </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" baseline="0"/>
+            <a:t> - manaully entered via insert equation (ink equation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" baseline="0"/>
+            <a:t> - evenly spaced to gridlines</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" baseline="0"/>
+            <a:t>- Excel camera is used to take a "live" picture which is then copied onto graphs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7CAA1E3-8AF8-44E6-BDF8-384CA87E936C}" name="tbl_GraphData" displayName="tbl_GraphData" ref="B7:E34" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="B7:E34" xr:uid="{A7CAA1E3-8AF8-44E6-BDF8-384CA87E936C}"/>
-  <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{CB89A46C-D511-4A20-A65C-DD895EDD1638}" name="Index">
-      <calculatedColumnFormula array="1">ROW()-ROW(tbl_GraphData[#Headers])-1</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="1" xr3:uid="{14372A7A-A7CB-443B-B3AE-3718244149DD}" name="Radians" dataCellStyle="Comma">
-      <calculatedColumnFormula>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B5C3165F-0EE5-4704-B4A3-4A49E01B3C5E}" name="Table2" displayName="Table2" ref="B5:C24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="4">
+  <autoFilter ref="B5:C24" xr:uid="{B5C3165F-0EE5-4704-B4A3-4A49E01B3C5E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4C2771CD-D8D5-494E-89F2-F4463C8A186F}" name="Radians" dataDxfId="6">
+      <calculatedColumnFormula array="1">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7D2C2F1A-525E-4910-B64A-015043FD0BBD}" name="Degrees" dataDxfId="1" dataCellStyle="Comma">
-      <calculatedColumnFormula>tbl_GraphData[[#This Row],[Radians]]/PI()*180</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{6C335BFB-9AC7-476D-830C-1CF9F64C9EAF}" name="y=sin(x)" dataDxfId="5">
+      <calculatedColumnFormula>SIN(Table2[[#This Row],[Radians]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{31E5FC97-4242-4F6A-9549-55898B30B135}" name="sin" dataDxfId="0">
-      <calculatedColumnFormula>SIN(tbl_GraphData[[#This Row],[Radians]])</calculatedColumnFormula>
+  </tableColumns>
+  <tableStyleInfo name="SpreadsheetBiStyle" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64F2C58B-AD3C-4AB6-89CC-D989792CAAD3}" name="Table24" displayName="Table24" ref="B29:C48" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="B29:C48" xr:uid="{64F2C58B-AD3C-4AB6-89CC-D989792CAAD3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{0DCA8770-CEDD-4D4A-9DAE-FFD5C31F738C}" name="Radians" dataDxfId="0">
+      <calculatedColumnFormula array="1">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{FAE9311E-3BAB-4706-9048-464346F24AAB}" name="y=cos(x)" dataDxfId="1">
+      <calculatedColumnFormula>COS(Table24[[#This Row],[Radians]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="SpreadsheetBiStyle" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3135,758 +5535,765 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A9F80A-97AA-44E9-93B4-1DF3BBDDCF60}">
-  <dimension ref="B2:N34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F6DE94-C457-442B-9D0C-C6A8A2BB55A0}">
+  <dimension ref="B2:C48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.90625" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.5">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K3" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6">
-        <f>-2 * PI()</f>
-        <v>-6.2831853071795862</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
-        <f>2* PI()</f>
-        <v>6.2831853071795862</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="K5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" cm="1">
-        <f t="array" ref="B8">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" cm="1">
+        <f t="array" ref="B6">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>-6.2831853071795862</v>
-      </c>
-      <c r="D8" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-360</v>
-      </c>
-      <c r="E8" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>2.45029690981724E-16</v>
+        <v>-6.5973445725385655</v>
+      </c>
+      <c r="C6" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>-0.30901699437494717</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" cm="1">
-        <f t="array" ref="B9">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>1</v>
-      </c>
-      <c r="C9" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" cm="1">
+        <f t="array" ref="B7">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>-5.7998633604734646</v>
-      </c>
-      <c r="D9" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-332.30769230769232</v>
-      </c>
-      <c r="E9" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.4647231720437684</v>
+        <v>-5.8643062867009474</v>
+      </c>
+      <c r="C7" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>0.40673664307580015</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B10" cm="1">
-        <f t="array" ref="B10">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>2</v>
-      </c>
-      <c r="C10" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" cm="1">
+        <f t="array" ref="B8">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>-5.3165414137673421</v>
-      </c>
-      <c r="D10" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-304.61538461538458</v>
-      </c>
-      <c r="E10" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.82298386589365657</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>10</v>
+        <v>-5.1312680008633285</v>
+      </c>
+      <c r="C8" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>0.91354545764260109</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B11" cm="1">
-        <f t="array" ref="B11">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>3</v>
-      </c>
-      <c r="C11" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" cm="1">
+        <f t="array" ref="B9">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>-4.8332194670612205</v>
-      </c>
-      <c r="D11" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-276.92307692307696</v>
-      </c>
-      <c r="E11" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.99270887409805397</v>
-      </c>
-      <c r="L11" t="s">
-        <v>8</v>
-      </c>
-      <c r="N11" t="str">
-        <f>_xlfn.UNICHAR(176)</f>
-        <v>°</v>
+        <v>-4.3982297150257104</v>
+      </c>
+      <c r="C9" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>0.95105651629515353</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B12" cm="1">
-        <f t="array" ref="B12">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>4</v>
-      </c>
-      <c r="C12" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" cm="1">
+        <f t="array" ref="B10">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>-4.349897520355098</v>
-      </c>
-      <c r="D12" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-249.23076923076923</v>
-      </c>
-      <c r="E12" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.93501624268541472</v>
-      </c>
-      <c r="L12" t="s">
-        <v>9</v>
-      </c>
-      <c r="N12" t="s">
-        <v>7</v>
+        <v>-3.6651914291880918</v>
+      </c>
+      <c r="C10" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>0.49999999999999972</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B13" cm="1">
-        <f t="array" ref="B13">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>5</v>
-      </c>
-      <c r="C13" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" cm="1">
+        <f t="array" ref="B11">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>-3.8665755736489764</v>
-      </c>
-      <c r="D13" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-221.53846153846155</v>
-      </c>
-      <c r="E13" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.6631226582407953</v>
+        <v>-2.9321531433504733</v>
+      </c>
+      <c r="C11" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>-0.20791169081775973</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B14" cm="1">
-        <f t="array" ref="B14">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>6</v>
-      </c>
-      <c r="C14" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" cm="1">
+        <f t="array" ref="B12">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>-3.3832536269428544</v>
-      </c>
-      <c r="D14" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-193.84615384615387</v>
-      </c>
-      <c r="E14" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.23931566428755788</v>
+        <v>-2.1991148575128552</v>
+      </c>
+      <c r="C12" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>-0.80901699437494745</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B15" cm="1">
-        <f t="array" ref="B15">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>7</v>
-      </c>
-      <c r="C15" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" cm="1">
+        <f t="array" ref="B13">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>-2.8999316802367323</v>
-      </c>
-      <c r="D15" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-166.15384615384616</v>
-      </c>
-      <c r="E15" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.23931566428755768</v>
+        <v>-1.4660765716752362</v>
+      </c>
+      <c r="C13" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>-0.99452189536827329</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B16" cm="1">
-        <f t="array" ref="B16">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>8</v>
-      </c>
-      <c r="C16" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" cm="1">
+        <f t="array" ref="B14">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>-2.4166097335306103</v>
-      </c>
-      <c r="D16" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-138.46153846153848</v>
-      </c>
-      <c r="E16" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.66312265824079519</v>
+        <v>-0.7330382858376181</v>
+      </c>
+      <c r="C14" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>-0.66913060635885802</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" cm="1">
-        <f t="array" ref="B17">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>9</v>
-      </c>
-      <c r="C17" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.ReturnValue
-)</f>
-        <v>-1.9332877868244882</v>
-      </c>
-      <c r="D17" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-110.76923076923077</v>
-      </c>
-      <c r="E17" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.93501624268541483</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" cm="1">
-        <f t="array" ref="B18">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>10</v>
-      </c>
-      <c r="C18" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.ReturnValue
-)</f>
-        <v>-1.4499658401183666</v>
-      </c>
-      <c r="D18" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-83.076923076923109</v>
-      </c>
-      <c r="E18" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.99270887409805408</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" cm="1">
-        <f t="array" ref="B19">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>11</v>
-      </c>
-      <c r="C19" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.ReturnValue
-)</f>
-        <v>-0.9666438934122441</v>
-      </c>
-      <c r="D19" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-55.384615384615387</v>
-      </c>
-      <c r="E19" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.82298386589365646</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B20" cm="1">
-        <f t="array" ref="B20">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>12</v>
-      </c>
-      <c r="C20" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.ReturnValue
-)</f>
-        <v>-0.4833219467061225</v>
-      </c>
-      <c r="D20" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>-27.692307692307718</v>
-      </c>
-      <c r="E20" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.46472317204376895</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B21" cm="1">
-        <f t="array" ref="B21">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>13</v>
-      </c>
-      <c r="C21" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B15" s="5" cm="1">
+        <f t="array" ref="B15">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
         <v>0</v>
       </c>
-      <c r="D21" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
+      <c r="C15" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0</v>
       </c>
-      <c r="E21" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B22" cm="1">
-        <f t="array" ref="B22">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>14</v>
-      </c>
-      <c r="C22" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B16" s="5" cm="1">
+        <f t="array" ref="B16">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>0.48332194670612161</v>
-      </c>
-      <c r="D22" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>27.692307692307669</v>
-      </c>
-      <c r="E22" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.46472317204376817</v>
+        <v>0.73303828583761899</v>
+      </c>
+      <c r="C16" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>0.66913060635885868</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B23" cm="1">
-        <f t="array" ref="B23">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>15</v>
-      </c>
-      <c r="C23" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="5" cm="1">
+        <f t="array" ref="B17">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>0.9666438934122441</v>
-      </c>
-      <c r="D23" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>55.384615384615387</v>
-      </c>
-      <c r="E23" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.82298386589365646</v>
+        <v>1.466076571675238</v>
+      </c>
+      <c r="C17" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>0.9945218953682734</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B24" cm="1">
-        <f t="array" ref="B24">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>16</v>
-      </c>
-      <c r="C24" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" cm="1">
+        <f t="array" ref="B18">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>1.4499658401183657</v>
-      </c>
-      <c r="D24" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>83.076923076923066</v>
-      </c>
-      <c r="E24" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.99270887409805397</v>
+        <v>2.1991148575128552</v>
+      </c>
+      <c r="C18" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>0.80901699437494745</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" cm="1">
-        <f t="array" ref="B25">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>17</v>
-      </c>
-      <c r="C25" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="5" cm="1">
+        <f t="array" ref="B19">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>1.9332877868244882</v>
-      </c>
-      <c r="D25" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>110.76923076923077</v>
-      </c>
-      <c r="E25" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.93501624268541483</v>
+        <v>2.9321531433504742</v>
+      </c>
+      <c r="C19" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>0.20791169081775887</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B26" cm="1">
-        <f t="array" ref="B26">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>18</v>
-      </c>
-      <c r="C26" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="5" cm="1">
+        <f t="array" ref="B20">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>2.4166097335306098</v>
-      </c>
-      <c r="D26" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>138.46153846153845</v>
-      </c>
-      <c r="E26" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.66312265824079553</v>
+        <v>3.6651914291880932</v>
+      </c>
+      <c r="C20" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>-0.50000000000000089</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B27" cm="1">
-        <f t="array" ref="B27">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>19</v>
-      </c>
-      <c r="C27" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="5" cm="1">
+        <f t="array" ref="B21">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>2.8999316802367314</v>
-      </c>
-      <c r="D27" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>166.15384615384613</v>
-      </c>
-      <c r="E27" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>0.23931566428755854</v>
+        <v>4.3982297150257104</v>
+      </c>
+      <c r="C21" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>-0.95105651629515353</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B28" cm="1">
-        <f t="array" ref="B28">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>20</v>
-      </c>
-      <c r="C28" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="5" cm="1">
+        <f t="array" ref="B22">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>3.383253626942853</v>
-      </c>
-      <c r="D28" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>193.84615384615381</v>
-      </c>
-      <c r="E28" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.23931566428755657</v>
+        <v>5.1312680008633293</v>
+      </c>
+      <c r="C22" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>-0.91354545764260076</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B29" cm="1">
-        <f t="array" ref="B29">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>21</v>
-      </c>
-      <c r="C29" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="5" cm="1">
+        <f t="array" ref="B23">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>3.8665755736489764</v>
-      </c>
-      <c r="D29" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>221.53846153846155</v>
-      </c>
-      <c r="E29" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.6631226582407953</v>
+        <v>5.8643062867009483</v>
+      </c>
+      <c r="C23" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>-0.40673664307579932</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" cm="1">
-        <f t="array" ref="B30">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>22</v>
-      </c>
-      <c r="C30" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="5" cm="1">
+        <f t="array" ref="B24">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>4.349897520355098</v>
-      </c>
-      <c r="D30" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>249.23076923076923</v>
-      </c>
-      <c r="E30" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.93501624268541472</v>
+        <v>6.5973445725385655</v>
+      </c>
+      <c r="C24" s="5">
+        <f>SIN(Table2[[#This Row],[Radians]])</f>
+        <v>0.30901699437494717</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B31" cm="1">
-        <f t="array" ref="B31">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>23</v>
-      </c>
-      <c r="C31" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" s="5" cm="1">
+        <f t="array" ref="B30">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>4.8332194670612196</v>
-      </c>
-      <c r="D31" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>276.92307692307691</v>
-      </c>
-      <c r="E31" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.99270887409805408</v>
+        <v>-6.5973445725385655</v>
+      </c>
+      <c r="C30" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>0.95105651629515364</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B32" cm="1">
-        <f t="array" ref="B32">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>24</v>
-      </c>
-      <c r="C32" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" s="5" cm="1">
+        <f t="array" ref="B31">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>5.3165414137673412</v>
-      </c>
-      <c r="D32" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>304.61538461538458</v>
-      </c>
-      <c r="E32" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.82298386589365702</v>
+        <v>-5.8643062867009474</v>
+      </c>
+      <c r="C31" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>0.91354545764260098</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" cm="1">
-        <f t="array" ref="B33">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>25</v>
-      </c>
-      <c r="C33" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="5" cm="1">
+        <f t="array" ref="B32">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>5.7998633604734628</v>
-      </c>
-      <c r="D33" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>332.30769230769226</v>
-      </c>
-      <c r="E33" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-0.46472317204376995</v>
+        <v>-5.1312680008633285</v>
+      </c>
+      <c r="C32" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>0.40673664307579976</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B34" cm="1">
-        <f t="array" ref="B34">ROW()-ROW(tbl_GraphData[#Headers])-1</f>
-        <v>26</v>
-      </c>
-      <c r="C34" s="8">
-        <f>_xlfn.LET(
-    _xlpm.Temp, -PI()+ (PI()*2/MAX(tbl_GraphData[Index])) * tbl_GraphData[[#This Row],[Index]],
-    _xlpm.NumberOfDataPoints, COUNTA(tbl_GraphData[Index]),
-    _xlpm.Increment, (Max_x_Value - Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
-    _xlpm.ReturnValue, Min_x_Value + _xlpm.Increment * tbl_GraphData[[#This Row],[Index]],
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" s="5" cm="1">
+        <f t="array" ref="B33">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
     _xlpm.ReturnValue
 )</f>
-        <v>6.2831853071795862</v>
-      </c>
-      <c r="D34" s="9">
-        <f>tbl_GraphData[[#This Row],[Radians]]/PI()*180</f>
-        <v>360</v>
-      </c>
-      <c r="E34" s="7">
-        <f>SIN(tbl_GraphData[[#This Row],[Radians]])</f>
-        <v>-2.45029690981724E-16</v>
+        <v>-4.3982297150257104</v>
+      </c>
+      <c r="C33" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>-0.30901699437494756</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" s="5" cm="1">
+        <f t="array" ref="B34">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-3.6651914291880918</v>
+      </c>
+      <c r="C34" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>-0.86602540378443882</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" s="5" cm="1">
+        <f t="array" ref="B35">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-2.9321531433504733</v>
+      </c>
+      <c r="C35" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>-0.97814760073380558</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" s="5" cm="1">
+        <f t="array" ref="B36">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-2.1991148575128552</v>
+      </c>
+      <c r="C36" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>-0.58778525229247303</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37" s="5" cm="1">
+        <f t="array" ref="B37">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-1.4660765716752362</v>
+      </c>
+      <c r="C37" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>0.10452846326765412</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38" s="5" cm="1">
+        <f t="array" ref="B38">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-0.7330382858376181</v>
+      </c>
+      <c r="C38" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>0.74314482547739447</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39" s="5" cm="1">
+        <f t="array" ref="B39">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B40" s="5" cm="1">
+        <f t="array" ref="B40">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>0.73303828583761899</v>
+      </c>
+      <c r="C40" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>0.74314482547739391</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B41" s="5" cm="1">
+        <f t="array" ref="B41">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>1.466076571675238</v>
+      </c>
+      <c r="C41" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>0.10452846326765235</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42" s="5" cm="1">
+        <f t="array" ref="B42">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>2.1991148575128552</v>
+      </c>
+      <c r="C42" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>-0.58778525229247303</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B43" s="5" cm="1">
+        <f t="array" ref="B43">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>2.9321531433504742</v>
+      </c>
+      <c r="C43" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>-0.97814760073380569</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B44" s="5" cm="1">
+        <f t="array" ref="B44">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>3.6651914291880932</v>
+      </c>
+      <c r="C44" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>-0.86602540378443815</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B45" s="5" cm="1">
+        <f t="array" ref="B45">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>4.3982297150257104</v>
+      </c>
+      <c r="C45" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>-0.30901699437494756</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B46" s="5" cm="1">
+        <f t="array" ref="B46">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>5.1312680008633293</v>
+      </c>
+      <c r="C46" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>0.40673664307580054</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B47" s="5" cm="1">
+        <f t="array" ref="B47">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>5.8643062867009483</v>
+      </c>
+      <c r="C47" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>0.91354545764260131</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48" s="5" cm="1">
+        <f t="array" ref="B48">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>6.5973445725385655</v>
+      </c>
+      <c r="C48" s="5">
+        <f>COS(Table24[[#This Row],[Radians]])</f>
+        <v>0.95105651629515364</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="2">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F6DE94-C457-442B-9D0C-C6A8A2BB55A0}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66B9F88-23CE-43CE-A4A9-785756259480}">
+  <dimension ref="B2:G31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="13.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="9" width="9.6328125" customWidth="1"/>
+    <col min="10" max="10" width="3.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add graphs to MA-T1
</commit_message>
<xml_diff>
--- a/WebsiteCreator/ImageCreators/ImageCreatorTrig.xlsx
+++ b/WebsiteCreator/ImageCreators/ImageCreatorTrig.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive\Documents_Charl\Computer_Technical\Programming_GitHub\AustralianSchoolMaths\WebsiteCreator\ImageCreators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B970BD-C69F-4D35-9903-8FF2864FF4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E281F5-D522-484C-8AF7-00271ED11745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StdAngles" sheetId="8" r:id="rId1"/>
     <sheet name="Graphs" sheetId="6" r:id="rId2"/>
-    <sheet name="RadianLables" sheetId="11" r:id="rId3"/>
+    <sheet name="RadianLabels" sheetId="11" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
@@ -23,8 +23,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="Max_x_Value" localSheetId="2">RadianLables!#REF!</definedName>
-    <definedName name="Min_x_Value" localSheetId="2">RadianLables!#REF!</definedName>
+    <definedName name="Max_x_Value" localSheetId="2">RadianLabels!#REF!</definedName>
+    <definedName name="Min_x_Value" localSheetId="2">RadianLabels!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Radians</t>
   </si>
@@ -88,6 +88,15 @@
   <si>
     <t>y=cos(x)</t>
   </si>
+  <si>
+    <t>y=tan(x)</t>
+  </si>
+  <si>
+    <t>Range option 1</t>
+  </si>
+  <si>
+    <t>Note that tan lines are manually inserted curves.  The actual graph is not shown as it gets nonsensically joined up, rather than showing asymptotes.</t>
+  </si>
 </sst>
 </file>
 
@@ -96,8 +105,16 @@
   <numFmts count="1">
     <numFmt numFmtId="171" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -133,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -145,12 +162,25 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="171" formatCode="0.00000"/>
     </dxf>
@@ -219,12 +249,17 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="SpreadsheetBiStyle" pivot="0" table="0" count="4" xr9:uid="{5890DF3A-0ABD-4274-8E00-EB660A947AED}">
-      <tableStyleElement type="wholeTable" dxfId="11"/>
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="secondRowStripe" dxfId="8"/>
+      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="secondRowStripe" dxfId="12"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FF5B9BD5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -252,7 +287,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.3137581699346403E-2"/>
+          <c:y val="1.4388383838383839E-2"/>
+          <c:w val="0.95245813074014052"/>
+          <c:h val="0.92086330935251803"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -604,6 +649,8 @@
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
+              <a:headEnd type="arrow" w="med" len="med"/>
+              <a:tailEnd type="arrow" w="med" len="med"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -738,6 +785,351 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.95105651629515364</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6EF5-4CF0-8ECB-DDB00B26DD02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="201277360"/>
+        <c:axId val="201274480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="201277360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:headEnd type="arrow" w="med" len="med"/>
+            <a:tailEnd type="arrow" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="201274480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="201274480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:headEnd type="arrow" w="med" len="med"/>
+            <a:tailEnd type="arrow" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="201277360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.3333333333333333E-2"/>
+          <c:y val="5.0925925925925916E-2"/>
+          <c:w val="0.93888888888888888"/>
+          <c:h val="0.89814814814814814"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Graphs!$B$56:$B$74</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-6.5973445725385655</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.8643062867009474</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.1312680008633285</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.3982297150257104</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.6651914291880918</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.9321531433504733</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.1991148575128552</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.4660765716752362</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.7330382858376181</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.73303828583761899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.466076571675238</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1991148575128552</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.9321531433504742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6651914291880932</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.3982297150257104</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.1312680008633293</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.8643062867009483</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.5973445725385655</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Graphs!$C$56:$C$74</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-0.32491969623290606</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4452286853085361</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2460367739042191</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.0776835371752518</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.5773502691896254</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.21255656167002254</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3763819204711738</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9.514364454222525</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.90040404429783938</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.90040404429784093</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.5143644542226884</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.3763819204711738</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.21255656167002163</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.57735026918962717</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.0776835371752518</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2.2460367739042137</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.44522868530853504</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.32491969623290606</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -953,6 +1345,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2024,6 +2456,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3476,15 +4424,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>98425</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>98424</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>403225</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>302424</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3495,7 +4443,9 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3514,15 +4464,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>12701</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:colOff>38101</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>120650</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>431800</xdr:colOff>
-          <xdr:row>15</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>596900</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -3537,7 +4487,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLables!$B$11:$J$13" spid="_x0000_s12308"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s12384"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3551,8 +4501,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="3295651" y="2336800"/>
-              <a:ext cx="3467099" cy="488950"/>
+              <a:off x="3321051" y="2565400"/>
+              <a:ext cx="4825999" cy="488950"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3578,15 +4528,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>136525</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>441325</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>308775</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>128750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3597,7 +4547,9 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3616,13 +4568,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>82550</xdr:colOff>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>36</xdr:row>
           <xdr:rowOff>50800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>501649</xdr:colOff>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>152400</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -3639,7 +4591,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLables!$B$11:$J$13" spid="_x0000_s12309"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s12385"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3653,8 +4605,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="3365500" y="6731000"/>
-              <a:ext cx="3467099" cy="488950"/>
+              <a:off x="3321050" y="6731000"/>
+              <a:ext cx="4991100" cy="488950"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3677,6 +4629,782 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>225425</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>429425</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>97000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C6B80A5-CAF7-94B5-0442-2B7ED796A5B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12708CD4-8B97-D575-3A12-7FB39CFC41B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6845300" y="10547350"/>
+          <a:ext cx="12700" cy="3213100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{867B2396-0FAC-4567-974D-F4A679750430}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5397500" y="10547350"/>
+          <a:ext cx="12700" cy="3213100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E34D7B1-7726-9488-FA3C-E1EED1078E60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8331200" y="10566400"/>
+          <a:ext cx="12700" cy="3213100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>406400</xdr:colOff>
+          <xdr:row>65</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>247650</xdr:colOff>
+          <xdr:row>68</xdr:row>
+          <xdr:rowOff>165100</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="17" name="Picture 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87032639-039D-43FD-8C9F-241629EAC553}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="RadianLabels!$C$22:$I$24" spid="_x0000_s12386"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="3689350" y="12039600"/>
+              <a:ext cx="5327650" cy="698500"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:noFill/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{413F28B7-681B-9434-F65F-D49ED9DA4FFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3854450" y="10585450"/>
+          <a:ext cx="12700" cy="3213100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>563329</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Freeform: Shape 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3516EA9A-6A4A-57F0-3A3A-5F37AABF9C86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7067550" y="10737850"/>
+          <a:ext cx="1045929" cy="2927350"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 1045929"/>
+            <a:gd name="connsiteY0" fmla="*/ 2927350 h 2927350"/>
+            <a:gd name="connsiteX1" fmla="*/ 19050 w 1045929"/>
+            <a:gd name="connsiteY1" fmla="*/ 2298700 h 2927350"/>
+            <a:gd name="connsiteX2" fmla="*/ 101600 w 1045929"/>
+            <a:gd name="connsiteY2" fmla="*/ 1955800 h 2927350"/>
+            <a:gd name="connsiteX3" fmla="*/ 419100 w 1045929"/>
+            <a:gd name="connsiteY3" fmla="*/ 1485900 h 2927350"/>
+            <a:gd name="connsiteX4" fmla="*/ 520700 w 1045929"/>
+            <a:gd name="connsiteY4" fmla="*/ 1352550 h 2927350"/>
+            <a:gd name="connsiteX5" fmla="*/ 857250 w 1045929"/>
+            <a:gd name="connsiteY5" fmla="*/ 984250 h 2927350"/>
+            <a:gd name="connsiteX6" fmla="*/ 1028700 w 1045929"/>
+            <a:gd name="connsiteY6" fmla="*/ 476250 h 2927350"/>
+            <a:gd name="connsiteX7" fmla="*/ 1041400 w 1045929"/>
+            <a:gd name="connsiteY7" fmla="*/ 0 h 2927350"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1045929" h="2927350">
+              <a:moveTo>
+                <a:pt x="0" y="2927350"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="1058" y="2693987"/>
+                <a:pt x="2117" y="2460625"/>
+                <a:pt x="19050" y="2298700"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="35983" y="2136775"/>
+                <a:pt x="34925" y="2091267"/>
+                <a:pt x="101600" y="1955800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="168275" y="1820333"/>
+                <a:pt x="349250" y="1586442"/>
+                <a:pt x="419100" y="1485900"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="488950" y="1385358"/>
+                <a:pt x="447675" y="1436158"/>
+                <a:pt x="520700" y="1352550"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="593725" y="1268942"/>
+                <a:pt x="772583" y="1130300"/>
+                <a:pt x="857250" y="984250"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="941917" y="838200"/>
+                <a:pt x="998008" y="640291"/>
+                <a:pt x="1028700" y="476250"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1059392" y="312209"/>
+                <a:pt x="1039283" y="81492"/>
+                <a:pt x="1041400" y="0"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="5B9BD5"/>
+          </a:solidFill>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-AU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>296629</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Freeform: Shape 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5340463A-BC96-4F23-9431-8DAF840EB93A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="10642600"/>
+          <a:ext cx="1045929" cy="2927350"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 1045929"/>
+            <a:gd name="connsiteY0" fmla="*/ 2927350 h 2927350"/>
+            <a:gd name="connsiteX1" fmla="*/ 19050 w 1045929"/>
+            <a:gd name="connsiteY1" fmla="*/ 2298700 h 2927350"/>
+            <a:gd name="connsiteX2" fmla="*/ 101600 w 1045929"/>
+            <a:gd name="connsiteY2" fmla="*/ 1955800 h 2927350"/>
+            <a:gd name="connsiteX3" fmla="*/ 419100 w 1045929"/>
+            <a:gd name="connsiteY3" fmla="*/ 1485900 h 2927350"/>
+            <a:gd name="connsiteX4" fmla="*/ 520700 w 1045929"/>
+            <a:gd name="connsiteY4" fmla="*/ 1352550 h 2927350"/>
+            <a:gd name="connsiteX5" fmla="*/ 857250 w 1045929"/>
+            <a:gd name="connsiteY5" fmla="*/ 984250 h 2927350"/>
+            <a:gd name="connsiteX6" fmla="*/ 1028700 w 1045929"/>
+            <a:gd name="connsiteY6" fmla="*/ 476250 h 2927350"/>
+            <a:gd name="connsiteX7" fmla="*/ 1041400 w 1045929"/>
+            <a:gd name="connsiteY7" fmla="*/ 0 h 2927350"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1045929" h="2927350">
+              <a:moveTo>
+                <a:pt x="0" y="2927350"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="1058" y="2693987"/>
+                <a:pt x="2117" y="2460625"/>
+                <a:pt x="19050" y="2298700"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="35983" y="2136775"/>
+                <a:pt x="34925" y="2091267"/>
+                <a:pt x="101600" y="1955800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="168275" y="1820333"/>
+                <a:pt x="349250" y="1586442"/>
+                <a:pt x="419100" y="1485900"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="488950" y="1385358"/>
+                <a:pt x="447675" y="1436158"/>
+                <a:pt x="520700" y="1352550"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="593725" y="1268942"/>
+                <a:pt x="772583" y="1130300"/>
+                <a:pt x="857250" y="984250"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="941917" y="838200"/>
+                <a:pt x="998008" y="640291"/>
+                <a:pt x="1028700" y="476250"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1059392" y="312209"/>
+                <a:pt x="1039283" y="81492"/>
+                <a:pt x="1041400" y="0"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="5B9BD5"/>
+          </a:solidFill>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-AU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>74379</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Freeform: Shape 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B164F23C-CABD-4F07-B84A-FF899CA07BBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4140200" y="10693400"/>
+          <a:ext cx="1045929" cy="2927350"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 1045929"/>
+            <a:gd name="connsiteY0" fmla="*/ 2927350 h 2927350"/>
+            <a:gd name="connsiteX1" fmla="*/ 19050 w 1045929"/>
+            <a:gd name="connsiteY1" fmla="*/ 2298700 h 2927350"/>
+            <a:gd name="connsiteX2" fmla="*/ 101600 w 1045929"/>
+            <a:gd name="connsiteY2" fmla="*/ 1955800 h 2927350"/>
+            <a:gd name="connsiteX3" fmla="*/ 419100 w 1045929"/>
+            <a:gd name="connsiteY3" fmla="*/ 1485900 h 2927350"/>
+            <a:gd name="connsiteX4" fmla="*/ 520700 w 1045929"/>
+            <a:gd name="connsiteY4" fmla="*/ 1352550 h 2927350"/>
+            <a:gd name="connsiteX5" fmla="*/ 857250 w 1045929"/>
+            <a:gd name="connsiteY5" fmla="*/ 984250 h 2927350"/>
+            <a:gd name="connsiteX6" fmla="*/ 1028700 w 1045929"/>
+            <a:gd name="connsiteY6" fmla="*/ 476250 h 2927350"/>
+            <a:gd name="connsiteX7" fmla="*/ 1041400 w 1045929"/>
+            <a:gd name="connsiteY7" fmla="*/ 0 h 2927350"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1045929" h="2927350">
+              <a:moveTo>
+                <a:pt x="0" y="2927350"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="1058" y="2693987"/>
+                <a:pt x="2117" y="2460625"/>
+                <a:pt x="19050" y="2298700"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="35983" y="2136775"/>
+                <a:pt x="34925" y="2091267"/>
+                <a:pt x="101600" y="1955800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="168275" y="1820333"/>
+                <a:pt x="349250" y="1586442"/>
+                <a:pt x="419100" y="1485900"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="488950" y="1385358"/>
+                <a:pt x="447675" y="1436158"/>
+                <a:pt x="520700" y="1352550"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="593725" y="1268942"/>
+                <a:pt x="772583" y="1130300"/>
+                <a:pt x="857250" y="984250"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="941917" y="838200"/>
+                <a:pt x="998008" y="640291"/>
+                <a:pt x="1028700" y="476250"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1059392" y="312209"/>
+                <a:pt x="1039283" y="81492"/>
+                <a:pt x="1041400" y="0"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="5B9BD5"/>
+          </a:solidFill>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-AU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3685,13 +5413,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>739775</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:colOff>669925</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>111125</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="325538" cy="316882"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -3705,7 +5433,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1692275" y="479425"/>
+              <a:off x="841375" y="2555875"/>
               <a:ext cx="325538" cy="316882"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3816,7 +5544,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -3830,7 +5558,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1692275" y="479425"/>
+              <a:off x="841375" y="2555875"/>
               <a:ext cx="325538" cy="316882"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3888,7 +5616,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>374650</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="302006" cy="172227"/>
@@ -4061,7 +5789,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="223907" cy="172227"/>
@@ -4223,7 +5951,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>149225</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="247440" cy="287643"/>
@@ -4414,7 +6142,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>863600</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>136525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="196850" cy="287643"/>
@@ -4592,14 +6320,14 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>908050</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="118494" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -4613,7 +6341,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5670550" y="549275"/>
+              <a:off x="4210050" y="2625725"/>
               <a:ext cx="118494" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4673,7 +6401,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -4687,7 +6415,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5670550" y="549275"/>
+              <a:off x="4210050" y="2625725"/>
               <a:ext cx="118494" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4745,7 +6473,7 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>869950</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="196592" cy="316882"/>
@@ -4936,7 +6664,7 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>850900</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>15875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="196592" cy="172227"/>
@@ -5187,14 +6915,1091 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="266419" cy="259302"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="TextBox 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{130CDD85-464D-EE91-817A-DDD0696DB653}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="854075" y="4010025"/>
+              <a:ext cx="266419" cy="259302"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="900">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="900" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="900" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="900" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜋</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="900" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="TextBox 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{130CDD85-464D-EE91-817A-DDD0696DB653}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="854075" y="4010025"/>
+              <a:ext cx="266419" cy="259302"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="900" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−3𝜋/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="183255" cy="140872"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="TextBox 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E37541E-B151-C1EF-AA15-0D5C6AE91455}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1530350" y="4079875"/>
+              <a:ext cx="183255" cy="140872"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="900">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="900" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜋</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="TextBox 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E37541E-B151-C1EF-AA15-0D5C6AE91455}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1530350" y="4079875"/>
+              <a:ext cx="183255" cy="140872"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="900" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−𝜋</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="202491" cy="235321"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="TextBox 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7E8B3C8-4D22-9A73-76FF-17869A459314}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2171700" y="4041775"/>
+              <a:ext cx="202491" cy="235321"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="900">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="900" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="900" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜋</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="900" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="TextBox 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7E8B3C8-4D22-9A73-76FF-17869A459314}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2171700" y="4041775"/>
+              <a:ext cx="202491" cy="235321"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="900" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−𝜋/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="196850" cy="235321"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="TextBox 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D554D47-5155-FDC2-5F80-7E0915D42D23}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3517900" y="4054475"/>
+              <a:ext cx="196850" cy="235321"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="900" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="900" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜋</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="900" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="TextBox 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D554D47-5155-FDC2-5F80-7E0915D42D23}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3517900" y="4054475"/>
+              <a:ext cx="196850" cy="235321"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="900" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜋/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="97014" cy="140872"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="17" name="TextBox 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{761AFE45-84C1-AEC0-7130-7141C706F8D3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4229100" y="4117975"/>
+              <a:ext cx="97014" cy="140872"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="900" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="accent3">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜋</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="17" name="TextBox 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{761AFE45-84C1-AEC0-7130-7141C706F8D3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4229100" y="4117975"/>
+              <a:ext cx="97014" cy="140872"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="900" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜋</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="160941" cy="259302"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="18" name="TextBox 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{397D174D-0B39-F9FA-C6C1-FC2A4D5C0606}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4902200" y="4029075"/>
+              <a:ext cx="160941" cy="259302"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="900" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="900">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="900" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜋</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="900" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="accent3">
+                                <a:lumMod val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="18" name="TextBox 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{397D174D-0B39-F9FA-C6C1-FC2A4D5C0606}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4902200" y="4029075"/>
+              <a:ext cx="160941" cy="259302"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-AU" sz="900" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>3𝜋/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B5C3165F-0EE5-4704-B4A3-4A49E01B3C5E}" name="Table2" displayName="Table2" ref="B5:C24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B5C3165F-0EE5-4704-B4A3-4A49E01B3C5E}" name="Table2" displayName="Table2" ref="B5:C24" totalsRowShown="0" headerRowDxfId="11" dataDxfId="8">
   <autoFilter ref="B5:C24" xr:uid="{B5C3165F-0EE5-4704-B4A3-4A49E01B3C5E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4C2771CD-D8D5-494E-89F2-F4463C8A186F}" name="Radians" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{4C2771CD-D8D5-494E-89F2-F4463C8A186F}" name="Radians" dataDxfId="10">
       <calculatedColumnFormula array="1">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5205,7 +8010,7 @@
     _xlpm.ReturnValue
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{6C335BFB-9AC7-476D-830C-1CF9F64C9EAF}" name="y=sin(x)" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{6C335BFB-9AC7-476D-830C-1CF9F64C9EAF}" name="y=sin(x)" dataDxfId="9">
       <calculatedColumnFormula>SIN(Table2[[#This Row],[Radians]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5214,10 +8019,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64F2C58B-AD3C-4AB6-89CC-D989792CAAD3}" name="Table24" displayName="Table24" ref="B29:C48" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64F2C58B-AD3C-4AB6-89CC-D989792CAAD3}" name="Table24" displayName="Table24" ref="B29:C48" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B29:C48" xr:uid="{64F2C58B-AD3C-4AB6-89CC-D989792CAAD3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0DCA8770-CEDD-4D4A-9DAE-FFD5C31F738C}" name="Radians" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{0DCA8770-CEDD-4D4A-9DAE-FFD5C31F738C}" name="Radians" dataDxfId="4">
       <calculatedColumnFormula array="1">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -5228,8 +8033,31 @@
     _xlpm.ReturnValue
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FAE9311E-3BAB-4706-9048-464346F24AAB}" name="y=cos(x)" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{FAE9311E-3BAB-4706-9048-464346F24AAB}" name="y=cos(x)" dataDxfId="5">
       <calculatedColumnFormula>COS(Table24[[#This Row],[Radians]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="SpreadsheetBiStyle" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2CF24BE7-5CC5-4D9D-8FBB-E4ECB332DBD8}" name="Table245" displayName="Table245" ref="B55:C74" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="B55:C74" xr:uid="{2CF24BE7-5CC5-4D9D-8FBB-E4ECB332DBD8}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{451D42AB-9FC4-4AFF-9932-706FE4AC6BAA}" name="Radians" dataDxfId="1">
+      <calculatedColumnFormula array="1">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{16415C2B-C18C-4A12-AA8E-81EC8FA77B11}" name="y=tan(x)" dataDxfId="0">
+      <calculatedColumnFormula>TAN(Table245[[#This Row],[Radians]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="SpreadsheetBiStyle" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5536,10 +8364,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F6DE94-C457-442B-9D0C-C6A8A2BB55A0}">
-  <dimension ref="B2:C48"/>
+  <dimension ref="B2:E74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="R75" sqref="R75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5550,7 +8378,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5563,7 +8391,7 @@
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="5" cm="1">
+      <c r="B6" s="6" cm="1">
         <f t="array" ref="B6">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5575,13 +8403,13 @@
 )</f>
         <v>-6.5973445725385655</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>-0.30901699437494717</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B7" s="5" cm="1">
+      <c r="B7" s="6" cm="1">
         <f t="array" ref="B7">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5593,13 +8421,13 @@
 )</f>
         <v>-5.8643062867009474</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0.40673664307580015</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B8" s="5" cm="1">
+      <c r="B8" s="6" cm="1">
         <f t="array" ref="B8">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5611,13 +8439,13 @@
 )</f>
         <v>-5.1312680008633285</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0.91354545764260109</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B9" s="5" cm="1">
+      <c r="B9" s="6" cm="1">
         <f t="array" ref="B9">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5629,13 +8457,13 @@
 )</f>
         <v>-4.3982297150257104</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0.95105651629515353</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B10" s="5" cm="1">
+      <c r="B10" s="6" cm="1">
         <f t="array" ref="B10">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5647,13 +8475,13 @@
 )</f>
         <v>-3.6651914291880918</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0.49999999999999972</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B11" s="5" cm="1">
+      <c r="B11" s="6" cm="1">
         <f t="array" ref="B11">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5665,13 +8493,13 @@
 )</f>
         <v>-2.9321531433504733</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>-0.20791169081775973</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B12" s="5" cm="1">
+      <c r="B12" s="6" cm="1">
         <f t="array" ref="B12">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5683,13 +8511,13 @@
 )</f>
         <v>-2.1991148575128552</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>-0.80901699437494745</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B13" s="5" cm="1">
+      <c r="B13" s="6" cm="1">
         <f t="array" ref="B13">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5701,13 +8529,13 @@
 )</f>
         <v>-1.4660765716752362</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>-0.99452189536827329</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B14" s="5" cm="1">
+      <c r="B14" s="6" cm="1">
         <f t="array" ref="B14">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5719,13 +8547,13 @@
 )</f>
         <v>-0.7330382858376181</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>-0.66913060635885802</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B15" s="5" cm="1">
+      <c r="B15" s="6" cm="1">
         <f t="array" ref="B15">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5737,13 +8565,13 @@
 )</f>
         <v>0</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B16" s="5" cm="1">
+      <c r="B16" s="6" cm="1">
         <f t="array" ref="B16">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5755,13 +8583,13 @@
 )</f>
         <v>0.73303828583761899</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0.66913060635885868</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="5" cm="1">
+      <c r="B17" s="6" cm="1">
         <f t="array" ref="B17">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5773,13 +8601,13 @@
 )</f>
         <v>1.466076571675238</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0.9945218953682734</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="5" cm="1">
+      <c r="B18" s="6" cm="1">
         <f t="array" ref="B18">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5791,13 +8619,13 @@
 )</f>
         <v>2.1991148575128552</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0.80901699437494745</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="5" cm="1">
+      <c r="B19" s="6" cm="1">
         <f t="array" ref="B19">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5809,13 +8637,13 @@
 )</f>
         <v>2.9321531433504742</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0.20791169081775887</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="5" cm="1">
+      <c r="B20" s="6" cm="1">
         <f t="array" ref="B20">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5827,13 +8655,13 @@
 )</f>
         <v>3.6651914291880932</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>-0.50000000000000089</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="5" cm="1">
+      <c r="B21" s="6" cm="1">
         <f t="array" ref="B21">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5845,13 +8673,13 @@
 )</f>
         <v>4.3982297150257104</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>-0.95105651629515353</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="5" cm="1">
+      <c r="B22" s="6" cm="1">
         <f t="array" ref="B22">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5863,13 +8691,13 @@
 )</f>
         <v>5.1312680008633293</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>-0.91354545764260076</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="5" cm="1">
+      <c r="B23" s="6" cm="1">
         <f t="array" ref="B23">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5881,13 +8709,13 @@
 )</f>
         <v>5.8643062867009483</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>-0.40673664307579932</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="5" cm="1">
+      <c r="B24" s="6" cm="1">
         <f t="array" ref="B24">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table2[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table2[Radians]),
@@ -5899,7 +8727,7 @@
 )</f>
         <v>6.5973445725385655</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="6">
         <f>SIN(Table2[[#This Row],[Radians]])</f>
         <v>0.30901699437494717</v>
       </c>
@@ -5913,7 +8741,7 @@
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B30" s="5" cm="1">
+      <c r="B30" s="6" cm="1">
         <f t="array" ref="B30">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -5925,13 +8753,13 @@
 )</f>
         <v>-6.5973445725385655</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>0.95105651629515364</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="5" cm="1">
+      <c r="B31" s="6" cm="1">
         <f t="array" ref="B31">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -5943,13 +8771,13 @@
 )</f>
         <v>-5.8643062867009474</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>0.91354545764260098</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="5" cm="1">
+      <c r="B32" s="6" cm="1">
         <f t="array" ref="B32">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -5961,13 +8789,13 @@
 )</f>
         <v>-5.1312680008633285</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>0.40673664307579976</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B33" s="5" cm="1">
+      <c r="B33" s="6" cm="1">
         <f t="array" ref="B33">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -5979,13 +8807,13 @@
 )</f>
         <v>-4.3982297150257104</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>-0.30901699437494756</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B34" s="5" cm="1">
+      <c r="B34" s="6" cm="1">
         <f t="array" ref="B34">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -5997,13 +8825,13 @@
 )</f>
         <v>-3.6651914291880918</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>-0.86602540378443882</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B35" s="5" cm="1">
+      <c r="B35" s="6" cm="1">
         <f t="array" ref="B35">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6015,13 +8843,13 @@
 )</f>
         <v>-2.9321531433504733</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>-0.97814760073380558</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B36" s="5" cm="1">
+      <c r="B36" s="6" cm="1">
         <f t="array" ref="B36">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6033,13 +8861,13 @@
 )</f>
         <v>-2.1991148575128552</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>-0.58778525229247303</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="5" cm="1">
+      <c r="B37" s="6" cm="1">
         <f t="array" ref="B37">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6051,13 +8879,13 @@
 )</f>
         <v>-1.4660765716752362</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>0.10452846326765412</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B38" s="5" cm="1">
+      <c r="B38" s="6" cm="1">
         <f t="array" ref="B38">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6069,13 +8897,13 @@
 )</f>
         <v>-0.7330382858376181</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>0.74314482547739447</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="5" cm="1">
+      <c r="B39" s="6" cm="1">
         <f t="array" ref="B39">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6087,13 +8915,13 @@
 )</f>
         <v>0</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="5" cm="1">
+      <c r="B40" s="6" cm="1">
         <f t="array" ref="B40">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6105,13 +8933,13 @@
 )</f>
         <v>0.73303828583761899</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>0.74314482547739391</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41" s="5" cm="1">
+      <c r="B41" s="6" cm="1">
         <f t="array" ref="B41">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6123,13 +8951,13 @@
 )</f>
         <v>1.466076571675238</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>0.10452846326765235</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="5" cm="1">
+      <c r="B42" s="6" cm="1">
         <f t="array" ref="B42">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6141,13 +8969,13 @@
 )</f>
         <v>2.1991148575128552</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>-0.58778525229247303</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="5" cm="1">
+      <c r="B43" s="6" cm="1">
         <f t="array" ref="B43">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6159,13 +8987,13 @@
 )</f>
         <v>2.9321531433504742</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>-0.97814760073380569</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="5" cm="1">
+      <c r="B44" s="6" cm="1">
         <f t="array" ref="B44">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6177,13 +9005,13 @@
 )</f>
         <v>3.6651914291880932</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>-0.86602540378443815</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="5" cm="1">
+      <c r="B45" s="6" cm="1">
         <f t="array" ref="B45">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6195,13 +9023,13 @@
 )</f>
         <v>4.3982297150257104</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>-0.30901699437494756</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="5" cm="1">
+      <c r="B46" s="6" cm="1">
         <f t="array" ref="B46">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6213,13 +9041,13 @@
 )</f>
         <v>5.1312680008633293</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>0.40673664307580054</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="5" cm="1">
+      <c r="B47" s="6" cm="1">
         <f t="array" ref="B47">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6231,13 +9059,13 @@
 )</f>
         <v>5.8643062867009483</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>0.91354545764260131</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="5" cm="1">
+      <c r="B48" s="6" cm="1">
         <f t="array" ref="B48">_xlfn.LET(
     _xlpm.Index, ROW()-ROW(Table24[#Headers])-1,
     _xlpm.NumberOfDataPoints, ROWS(Table24[Radians]),
@@ -6249,28 +9077,384 @@
 )</f>
         <v>6.5973445725385655</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="6">
         <f>COS(Table24[[#This Row],[Radians]])</f>
         <v>0.95105651629515364</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B55" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B56" s="6" cm="1">
+        <f t="array" ref="B56">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-6.5973445725385655</v>
+      </c>
+      <c r="C56" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>-0.32491969623290606</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B57" s="6" cm="1">
+        <f t="array" ref="B57">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-5.8643062867009474</v>
+      </c>
+      <c r="C57" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>0.4452286853085361</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B58" s="6" cm="1">
+        <f t="array" ref="B58">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-5.1312680008633285</v>
+      </c>
+      <c r="C58" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>2.2460367739042191</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B59" s="6" cm="1">
+        <f t="array" ref="B59">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-4.3982297150257104</v>
+      </c>
+      <c r="C59" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>-3.0776835371752518</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B60" s="6" cm="1">
+        <f t="array" ref="B60">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-3.6651914291880918</v>
+      </c>
+      <c r="C60" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>-0.5773502691896254</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B61" s="6" cm="1">
+        <f t="array" ref="B61">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-2.9321531433504733</v>
+      </c>
+      <c r="C61" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>0.21255656167002254</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B62" s="6" cm="1">
+        <f t="array" ref="B62">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-2.1991148575128552</v>
+      </c>
+      <c r="C62" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>1.3763819204711738</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B63" s="6" cm="1">
+        <f t="array" ref="B63">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-1.4660765716752362</v>
+      </c>
+      <c r="C63" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>-9.514364454222525</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B64" s="6" cm="1">
+        <f t="array" ref="B64">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>-0.7330382858376181</v>
+      </c>
+      <c r="C64" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>-0.90040404429783938</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B65" s="6" cm="1">
+        <f t="array" ref="B65">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>0</v>
+      </c>
+      <c r="C65" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B66" s="6" cm="1">
+        <f t="array" ref="B66">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>0.73303828583761899</v>
+      </c>
+      <c r="C66" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>0.90040404429784093</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B67" s="6" cm="1">
+        <f t="array" ref="B67">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>1.466076571675238</v>
+      </c>
+      <c r="C67" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>9.5143644542226884</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B68" s="6" cm="1">
+        <f t="array" ref="B68">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>2.1991148575128552</v>
+      </c>
+      <c r="C68" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>-1.3763819204711738</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B69" s="6" cm="1">
+        <f t="array" ref="B69">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>2.9321531433504742</v>
+      </c>
+      <c r="C69" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>-0.21255656167002163</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B70" s="6" cm="1">
+        <f t="array" ref="B70">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>3.6651914291880932</v>
+      </c>
+      <c r="C70" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>0.57735026918962717</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B71" s="6" cm="1">
+        <f t="array" ref="B71">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>4.3982297150257104</v>
+      </c>
+      <c r="C71" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>3.0776835371752518</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B72" s="6" cm="1">
+        <f t="array" ref="B72">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>5.1312680008633293</v>
+      </c>
+      <c r="C72" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>-2.2460367739042137</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B73" s="6" cm="1">
+        <f t="array" ref="B73">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>5.8643062867009483</v>
+      </c>
+      <c r="C73" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>-0.44522868530853504</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B74" s="6" cm="1">
+        <f t="array" ref="B74">_xlfn.LET(
+    _xlpm.Index, ROW()-ROW(Table245[#Headers])-1,
+    _xlpm.NumberOfDataPoints, ROWS(Table245[Radians]),
+    _xlpm.Min_x_Value, -2.1 * PI(),
+    _xlpm.Max_X_Value, 2.1* PI(),
+    _xlpm.Increment, (_xlpm.Max_X_Value - _xlpm.Min_x_Value) / (_xlpm.NumberOfDataPoints-1),
+    _xlpm.ReturnValue, _xlpm.Min_x_Value + _xlpm.Increment * _xlpm.Index,
+    _xlpm.ReturnValue
+)</f>
+        <v>6.5973445725385655</v>
+      </c>
+      <c r="C74" s="6">
+        <f>TAN(Table245[[#This Row],[Radians]])</f>
+        <v>0.32491969623290606</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66B9F88-23CE-43CE-A4A9-785756259480}">
-  <dimension ref="B2:G31"/>
+  <dimension ref="B2:G34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6281,12 +9465,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G31" t="s">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G34" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add amplitude period phase centreto MA-T1
</commit_message>
<xml_diff>
--- a/WebsiteCreator/ImageCreators/ImageCreatorTrig.xlsx
+++ b/WebsiteCreator/ImageCreators/ImageCreatorTrig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive\Documents_Charl\Computer_Technical\Programming_GitHub\AustralianSchoolMaths\WebsiteCreator\ImageCreators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E281F5-D522-484C-8AF7-00271ED11745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC4FC0F-FE80-4AAD-81F9-69A0F5639B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4487,7 +4487,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s12384"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s12387"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4591,7 +4591,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s12385"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s12388"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4852,7 +4852,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$C$22:$I$24" spid="_x0000_s12386"/>
+                  <a14:cameraTool cellRange="RadianLabels!$C$22:$I$24" spid="_x0000_s12389"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -8367,7 +8367,7 @@
   <dimension ref="B2:E74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="R75" sqref="R75"/>
+      <selection activeCell="S72" sqref="S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
MA-T2 work in progress
</commit_message>
<xml_diff>
--- a/WebsiteCreator/ImageCreators/ImageCreatorTrig.xlsx
+++ b/WebsiteCreator/ImageCreators/ImageCreatorTrig.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/491e2628f664332b/Documents_Charl/Computer_Technical/Programming_GitHub/AustralianSchoolMaths/WebsiteCreator/ImageCreators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="350" documentId="13_ncr:1_{5DC4FC0F-FE80-4AAD-81F9-69A0F5639B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{164FBFD0-4AA0-431F-B2CF-DAE94FE30E19}"/>
+  <xr:revisionPtr revIDLastSave="375" documentId="13_ncr:1_{5DC4FC0F-FE80-4AAD-81F9-69A0F5639B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C335828B-3F95-4758-977D-2F4D5F955F08}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StdAngles" sheetId="8" r:id="rId1"/>
-    <sheet name="Graphs" sheetId="6" r:id="rId2"/>
-    <sheet name="RadianLabels" sheetId="11" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="CompAngles" sheetId="5" r:id="rId2"/>
+    <sheet name="Graphs" sheetId="6" r:id="rId3"/>
+    <sheet name="RadianLabels" sheetId="11" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="Max_x_Value" localSheetId="2">RadianLabels!#REF!</definedName>
-    <definedName name="Min_x_Value" localSheetId="2">RadianLabels!#REF!</definedName>
+    <definedName name="Max_x_Value" localSheetId="3">RadianLabels!#REF!</definedName>
+    <definedName name="Min_x_Value" localSheetId="3">RadianLabels!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Radians</t>
   </si>
@@ -105,6 +105,21 @@
   </si>
   <si>
     <t>y=cot(x)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Complementary Angles</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -174,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -190,6 +205,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7261,6 +7282,553 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>92075</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Triangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A0112BE-1B84-4F6C-947C-5DC8A633712B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="701675" y="974725"/>
+          <a:ext cx="2222500" cy="1962150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rtTriangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-AU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C74B0C3A-1408-B12C-60D5-300C9ACC99DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="692150" y="2603500"/>
+          <a:ext cx="400050" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C3849E4-4ECB-8AFC-C40D-C6382498795B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1092200" y="2603500"/>
+          <a:ext cx="0" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>511175</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="183512" cy="175369"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D6D1FF7-8FF1-1BCA-982C-4636D301FE81}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2339975" y="2705100"/>
+              <a:ext cx="183512" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="1100">
+                            <a:solidFill>
+                              <a:srgbClr val="836967"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜃</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D6D1FF7-8FF1-1BCA-982C-4636D301FE81}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2339975" y="2705100"/>
+              <a:ext cx="183512" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜃</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:srgbClr val="836967"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="573234" cy="175369"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62B95C48-979A-9650-B829-758FB3048245}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="752475" y="1504950"/>
+              <a:ext cx="573234" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="1100">
+                            <a:solidFill>
+                              <a:srgbClr val="836967"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>90</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-AU" sz="1100" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:srgbClr val="836967"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜃</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-AU" sz="1100" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-AU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62B95C48-979A-9650-B829-758FB3048245}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="752475" y="1504950"/>
+              <a:ext cx="573234" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>90</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:srgbClr val="836967"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0−𝜃</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:srgbClr val="836967"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-AU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>98424</xdr:colOff>
       <xdr:row>5</xdr:row>
@@ -7325,7 +7893,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13002"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13074"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7429,7 +7997,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13003"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13075"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -7690,7 +8258,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$C$22:$I$24" spid="_x0000_s13004"/>
+                  <a14:cameraTool cellRange="RadianLabels!$C$22:$I$24" spid="_x0000_s13076"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -8309,7 +8877,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13005"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13077"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -10407,7 +10975,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13006"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13078"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -10617,7 +11185,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13007"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13079"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13918,7 +14486,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13008"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13080"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13978,7 +14546,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13009"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13081"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14038,7 +14606,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$C$22:$I$24" spid="_x0000_s13010"/>
+                  <a14:cameraTool cellRange="RadianLabels!$C$22:$I$24" spid="_x0000_s13082"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14110,7 +14678,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13011"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13083"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14170,7 +14738,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13012"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13084"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14230,7 +14798,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13013"/>
+                  <a14:cameraTool cellRange="RadianLabels!$B$14:$J$16" spid="_x0000_s13085"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14900,7 +15468,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -17892,10 +18460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F62744-82D2-4A3B-A267-D2E377FE4A99}">
-  <dimension ref="D11:F35"/>
+  <dimension ref="D11:L35"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17906,14 +18474,19 @@
       </c>
     </row>
     <row r="16" spans="6:6" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.35">
       <c r="E17" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.35">
       <c r="D26" s="2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="L28" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.35">
@@ -17928,10 +18501,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE32DF4-00D4-4D42-A1CC-D0A572DCF0E2}">
+  <dimension ref="A3:D18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F6DE94-C457-442B-9D0C-C6A8A2BB55A0}">
   <dimension ref="B2:E156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A129" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="V147" sqref="V147"/>
     </sheetView>
   </sheetViews>
@@ -20102,7 +20709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66B9F88-23CE-43CE-A4A9-785756259480}">
   <dimension ref="B2:G34"/>
   <sheetViews>
@@ -20141,20 +20748,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE32DF4-00D4-4D42-A1CC-D0A572DCF0E2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>